<commit_message>
WIP: local changes before pulling from remote
</commit_message>
<xml_diff>
--- a/data/data_set/SI_DS2_AvoidanceCostCurve_CombinedUnits.xlsx
+++ b/data/data_set/SI_DS2_AvoidanceCostCurve_CombinedUnits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ede013533779f48/PhD/PhD Programe UofC/LCA/Paper 01/SI Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ede013533779f48/PhD/PhD Programe UofC/LCA/Paper 01/github/carbon-capture-refinery-analysis/data/data_set/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{9CB230B7-880A-40BC-9E80-0DB4967BCB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7822F6C-2302-4DF0-9580-A9A54687B1F4}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{9CB230B7-880A-40BC-9E80-0DB4967BCB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C82274F-6050-43D9-9D2D-3ECEEF7E3481}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="16440" windowHeight="28320" xr2:uid="{4E6F5E44-B7F5-4DB9-928D-4648349E6FFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E6F5E44-B7F5-4DB9-928D-4648349E6FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet4" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1841,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K36" xr:uid="{9F82B3DD-ACE5-4329-A2F2-A17003F3E675}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>